<commit_message>
chore: update Excel file for event management data
</commit_message>
<xml_diff>
--- a/public/xlsx/736067c4-bd56-4c2e-8e0e-6bd9cfa9f39c.xlsx
+++ b/public/xlsx/736067c4-bd56-4c2e-8e0e-6bd9cfa9f39c.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Página1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="config" sheetId="2" r:id="rId5"/>
+    <sheet state="hidden" name="config" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>LISTA DE INSCRIÇÕES</t>
   </si>
@@ -84,6 +84,9 @@
     <t>Normal</t>
   </si>
   <si>
+    <t>Participação</t>
+  </si>
+  <si>
     <t>Serviço</t>
   </si>
   <si>
@@ -98,7 +101,7 @@
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/MM/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -147,6 +150,11 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -174,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -189,7 +197,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -198,19 +208,20 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -427,7 +438,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4.0" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B6" sqref="B6" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
@@ -436,7 +450,6 @@
     <col customWidth="1" min="3" max="3" width="29.75"/>
     <col customWidth="1" min="4" max="4" width="22.0"/>
     <col customWidth="1" min="5" max="5" width="17.75"/>
-    <col customWidth="1" min="6" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -459,7 +472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" ht="32.25" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -515,7 +528,7 @@
         <v>3.0</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="12">
@@ -528,7 +541,7 @@
         <v>4.0</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="14"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="12">
@@ -541,7 +554,7 @@
         <v>5.0</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="14"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="12">
@@ -554,7 +567,7 @@
         <v>6.0</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="14"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="12">
@@ -567,7 +580,7 @@
         <v>7.0</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="14"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="12">
@@ -580,7 +593,7 @@
         <v>8.0</v>
       </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="14"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="12">
@@ -593,7 +606,7 @@
         <v>9.0</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="14"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="12">
@@ -606,7 +619,7 @@
         <v>10.0</v>
       </c>
       <c r="B15" s="9"/>
-      <c r="C15" s="14"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="12">
@@ -619,7 +632,7 @@
         <v>11.0</v>
       </c>
       <c r="B16" s="9"/>
-      <c r="C16" s="14"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="12">
@@ -632,7 +645,7 @@
         <v>12.0</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="14"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="12">
@@ -645,7 +658,7 @@
         <v>13.0</v>
       </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="14"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="12">
@@ -658,7 +671,7 @@
         <v>14.0</v>
       </c>
       <c r="B19" s="9"/>
-      <c r="C19" s="14"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="12">
@@ -671,7 +684,7 @@
         <v>15.0</v>
       </c>
       <c r="B20" s="9"/>
-      <c r="C20" s="14"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="12">
@@ -684,7 +697,7 @@
         <v>16.0</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="14"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="12">
@@ -697,7 +710,7 @@
         <v>17.0</v>
       </c>
       <c r="B22" s="9"/>
-      <c r="C22" s="14"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="12">
@@ -710,7 +723,7 @@
         <v>18.0</v>
       </c>
       <c r="B23" s="9"/>
-      <c r="C23" s="14"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="12">
@@ -723,7 +736,7 @@
         <v>19.0</v>
       </c>
       <c r="B24" s="9"/>
-      <c r="C24" s="14"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="12">
@@ -736,7 +749,7 @@
         <v>20.0</v>
       </c>
       <c r="B25" s="9"/>
-      <c r="C25" s="14"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="12">
@@ -749,7 +762,7 @@
         <v>21.0</v>
       </c>
       <c r="B26" s="9"/>
-      <c r="C26" s="14"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="12">
@@ -762,7 +775,7 @@
         <v>22.0</v>
       </c>
       <c r="B27" s="9"/>
-      <c r="C27" s="14"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="12">
@@ -775,7 +788,7 @@
         <v>23.0</v>
       </c>
       <c r="B28" s="9"/>
-      <c r="C28" s="14"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="12">
@@ -788,7 +801,7 @@
         <v>24.0</v>
       </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="14"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="12">
@@ -801,7 +814,7 @@
         <v>25.0</v>
       </c>
       <c r="B30" s="9"/>
-      <c r="C30" s="14"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="12">
@@ -814,7 +827,7 @@
         <v>26.0</v>
       </c>
       <c r="B31" s="9"/>
-      <c r="C31" s="14"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="12">
@@ -827,7 +840,7 @@
         <v>27.0</v>
       </c>
       <c r="B32" s="9"/>
-      <c r="C32" s="14"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
       <c r="F32" s="12">
@@ -840,7 +853,7 @@
         <v>28.0</v>
       </c>
       <c r="B33" s="9"/>
-      <c r="C33" s="14"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="12">
@@ -853,7 +866,7 @@
         <v>29.0</v>
       </c>
       <c r="B34" s="9"/>
-      <c r="C34" s="14"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="12">
@@ -866,7 +879,7 @@
         <v>30.0</v>
       </c>
       <c r="B35" s="9"/>
-      <c r="C35" s="14"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
       <c r="F35" s="12">
@@ -879,7 +892,7 @@
         <v>31.0</v>
       </c>
       <c r="B36" s="9"/>
-      <c r="C36" s="14"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
       <c r="F36" s="12">
@@ -892,7 +905,7 @@
         <v>32.0</v>
       </c>
       <c r="B37" s="9"/>
-      <c r="C37" s="14"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="12">
@@ -905,7 +918,7 @@
         <v>33.0</v>
       </c>
       <c r="B38" s="9"/>
-      <c r="C38" s="14"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="12">
@@ -918,7 +931,7 @@
         <v>34.0</v>
       </c>
       <c r="B39" s="9"/>
-      <c r="C39" s="14"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="12">
@@ -931,7 +944,7 @@
         <v>35.0</v>
       </c>
       <c r="B40" s="9"/>
-      <c r="C40" s="14"/>
+      <c r="C40" s="10"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="12">
@@ -944,7 +957,7 @@
         <v>36.0</v>
       </c>
       <c r="B41" s="9"/>
-      <c r="C41" s="14"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="12">
@@ -957,7 +970,7 @@
         <v>37.0</v>
       </c>
       <c r="B42" s="9"/>
-      <c r="C42" s="14"/>
+      <c r="C42" s="10"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
       <c r="F42" s="12">
@@ -970,7 +983,7 @@
         <v>38.0</v>
       </c>
       <c r="B43" s="9"/>
-      <c r="C43" s="14"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="12">
@@ -983,7 +996,7 @@
         <v>39.0</v>
       </c>
       <c r="B44" s="9"/>
-      <c r="C44" s="14"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" s="12">
@@ -996,7 +1009,7 @@
         <v>40.0</v>
       </c>
       <c r="B45" s="9"/>
-      <c r="C45" s="14"/>
+      <c r="C45" s="10"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="12">
@@ -1009,7 +1022,7 @@
         <v>41.0</v>
       </c>
       <c r="B46" s="9"/>
-      <c r="C46" s="14"/>
+      <c r="C46" s="10"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="12">
@@ -1022,7 +1035,7 @@
         <v>42.0</v>
       </c>
       <c r="B47" s="9"/>
-      <c r="C47" s="14"/>
+      <c r="C47" s="10"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="12">
@@ -1035,7 +1048,7 @@
         <v>43.0</v>
       </c>
       <c r="B48" s="9"/>
-      <c r="C48" s="14"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="12">
@@ -1048,7 +1061,7 @@
         <v>44.0</v>
       </c>
       <c r="B49" s="9"/>
-      <c r="C49" s="14"/>
+      <c r="C49" s="10"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
       <c r="F49" s="12">
@@ -1061,7 +1074,7 @@
         <v>45.0</v>
       </c>
       <c r="B50" s="9"/>
-      <c r="C50" s="14"/>
+      <c r="C50" s="10"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
       <c r="F50" s="12">
@@ -1074,7 +1087,7 @@
         <v>46.0</v>
       </c>
       <c r="B51" s="9"/>
-      <c r="C51" s="14"/>
+      <c r="C51" s="10"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="12">
@@ -1087,7 +1100,7 @@
         <v>47.0</v>
       </c>
       <c r="B52" s="9"/>
-      <c r="C52" s="14"/>
+      <c r="C52" s="10"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="12">
@@ -1100,7 +1113,7 @@
         <v>48.0</v>
       </c>
       <c r="B53" s="9"/>
-      <c r="C53" s="14"/>
+      <c r="C53" s="10"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
       <c r="F53" s="12">
@@ -1113,7 +1126,7 @@
         <v>49.0</v>
       </c>
       <c r="B54" s="9"/>
-      <c r="C54" s="14"/>
+      <c r="C54" s="10"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="12">
@@ -1126,7 +1139,7 @@
         <v>50.0</v>
       </c>
       <c r="B55" s="9"/>
-      <c r="C55" s="14"/>
+      <c r="C55" s="10"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
       <c r="F55" s="12">
@@ -1139,7 +1152,7 @@
         <v>51.0</v>
       </c>
       <c r="B56" s="9"/>
-      <c r="C56" s="14"/>
+      <c r="C56" s="10"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="12">
@@ -1152,7 +1165,7 @@
         <v>52.0</v>
       </c>
       <c r="B57" s="9"/>
-      <c r="C57" s="14"/>
+      <c r="C57" s="10"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
       <c r="F57" s="12">
@@ -1165,7 +1178,7 @@
         <v>53.0</v>
       </c>
       <c r="B58" s="9"/>
-      <c r="C58" s="14"/>
+      <c r="C58" s="10"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
       <c r="F58" s="12">
@@ -1178,7 +1191,7 @@
         <v>54.0</v>
       </c>
       <c r="B59" s="9"/>
-      <c r="C59" s="14"/>
+      <c r="C59" s="10"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="12">
@@ -1191,7 +1204,7 @@
         <v>55.0</v>
       </c>
       <c r="B60" s="9"/>
-      <c r="C60" s="14"/>
+      <c r="C60" s="10"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="12">
@@ -1204,7 +1217,7 @@
         <v>56.0</v>
       </c>
       <c r="B61" s="9"/>
-      <c r="C61" s="14"/>
+      <c r="C61" s="10"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="12">
@@ -1217,7 +1230,7 @@
         <v>57.0</v>
       </c>
       <c r="B62" s="9"/>
-      <c r="C62" s="14"/>
+      <c r="C62" s="10"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
       <c r="F62" s="12">
@@ -1230,7 +1243,7 @@
         <v>58.0</v>
       </c>
       <c r="B63" s="9"/>
-      <c r="C63" s="14"/>
+      <c r="C63" s="10"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
       <c r="F63" s="12">
@@ -1243,7 +1256,7 @@
         <v>59.0</v>
       </c>
       <c r="B64" s="9"/>
-      <c r="C64" s="14"/>
+      <c r="C64" s="10"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
       <c r="F64" s="12">
@@ -1256,7 +1269,7 @@
         <v>60.0</v>
       </c>
       <c r="B65" s="9"/>
-      <c r="C65" s="14"/>
+      <c r="C65" s="10"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
       <c r="F65" s="12">
@@ -1269,7 +1282,7 @@
         <v>61.0</v>
       </c>
       <c r="B66" s="9"/>
-      <c r="C66" s="14"/>
+      <c r="C66" s="10"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
       <c r="F66" s="12">
@@ -1282,7 +1295,7 @@
         <v>62.0</v>
       </c>
       <c r="B67" s="9"/>
-      <c r="C67" s="14"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
       <c r="F67" s="12">
@@ -1295,7 +1308,7 @@
         <v>63.0</v>
       </c>
       <c r="B68" s="9"/>
-      <c r="C68" s="14"/>
+      <c r="C68" s="10"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="12">
@@ -1308,7 +1321,7 @@
         <v>64.0</v>
       </c>
       <c r="B69" s="9"/>
-      <c r="C69" s="14"/>
+      <c r="C69" s="10"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
       <c r="F69" s="12">
@@ -1321,7 +1334,7 @@
         <v>65.0</v>
       </c>
       <c r="B70" s="9"/>
-      <c r="C70" s="14"/>
+      <c r="C70" s="10"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="12">
@@ -1334,7 +1347,7 @@
         <v>66.0</v>
       </c>
       <c r="B71" s="9"/>
-      <c r="C71" s="14"/>
+      <c r="C71" s="10"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="12">
@@ -1347,7 +1360,7 @@
         <v>67.0</v>
       </c>
       <c r="B72" s="9"/>
-      <c r="C72" s="14"/>
+      <c r="C72" s="10"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
       <c r="F72" s="12">
@@ -1360,7 +1373,7 @@
         <v>68.0</v>
       </c>
       <c r="B73" s="9"/>
-      <c r="C73" s="14"/>
+      <c r="C73" s="10"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
       <c r="F73" s="12">
@@ -1373,7 +1386,7 @@
         <v>69.0</v>
       </c>
       <c r="B74" s="9"/>
-      <c r="C74" s="14"/>
+      <c r="C74" s="10"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
       <c r="F74" s="12">
@@ -1386,7 +1399,7 @@
         <v>70.0</v>
       </c>
       <c r="B75" s="9"/>
-      <c r="C75" s="14"/>
+      <c r="C75" s="10"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
       <c r="F75" s="12">
@@ -1399,7 +1412,7 @@
         <v>71.0</v>
       </c>
       <c r="B76" s="9"/>
-      <c r="C76" s="14"/>
+      <c r="C76" s="10"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
       <c r="F76" s="12">
@@ -1412,7 +1425,7 @@
         <v>72.0</v>
       </c>
       <c r="B77" s="9"/>
-      <c r="C77" s="14"/>
+      <c r="C77" s="10"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
       <c r="F77" s="12">
@@ -1425,7 +1438,7 @@
         <v>73.0</v>
       </c>
       <c r="B78" s="9"/>
-      <c r="C78" s="14"/>
+      <c r="C78" s="10"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
       <c r="F78" s="12">
@@ -1438,7 +1451,7 @@
         <v>74.0</v>
       </c>
       <c r="B79" s="9"/>
-      <c r="C79" s="14"/>
+      <c r="C79" s="10"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
       <c r="F79" s="12">
@@ -1451,7 +1464,7 @@
         <v>75.0</v>
       </c>
       <c r="B80" s="9"/>
-      <c r="C80" s="14"/>
+      <c r="C80" s="10"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="12">
@@ -1464,7 +1477,7 @@
         <v>76.0</v>
       </c>
       <c r="B81" s="9"/>
-      <c r="C81" s="14"/>
+      <c r="C81" s="10"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
       <c r="F81" s="12">
@@ -1477,7 +1490,7 @@
         <v>77.0</v>
       </c>
       <c r="B82" s="9"/>
-      <c r="C82" s="14"/>
+      <c r="C82" s="10"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
       <c r="F82" s="12">
@@ -1490,7 +1503,7 @@
         <v>78.0</v>
       </c>
       <c r="B83" s="9"/>
-      <c r="C83" s="14"/>
+      <c r="C83" s="10"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
       <c r="F83" s="12">
@@ -1503,7 +1516,7 @@
         <v>79.0</v>
       </c>
       <c r="B84" s="9"/>
-      <c r="C84" s="14"/>
+      <c r="C84" s="10"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
       <c r="F84" s="12">
@@ -1516,7 +1529,7 @@
         <v>80.0</v>
       </c>
       <c r="B85" s="9"/>
-      <c r="C85" s="14"/>
+      <c r="C85" s="10"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
       <c r="F85" s="12">
@@ -1529,7 +1542,7 @@
         <v>81.0</v>
       </c>
       <c r="B86" s="9"/>
-      <c r="C86" s="14"/>
+      <c r="C86" s="10"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
       <c r="F86" s="12">
@@ -1542,7 +1555,7 @@
         <v>82.0</v>
       </c>
       <c r="B87" s="9"/>
-      <c r="C87" s="14"/>
+      <c r="C87" s="10"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
       <c r="F87" s="12">
@@ -1555,7 +1568,7 @@
         <v>83.0</v>
       </c>
       <c r="B88" s="9"/>
-      <c r="C88" s="14"/>
+      <c r="C88" s="10"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
       <c r="F88" s="12">
@@ -1568,7 +1581,7 @@
         <v>84.0</v>
       </c>
       <c r="B89" s="9"/>
-      <c r="C89" s="14"/>
+      <c r="C89" s="10"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
       <c r="F89" s="12">
@@ -1581,7 +1594,7 @@
         <v>85.0</v>
       </c>
       <c r="B90" s="9"/>
-      <c r="C90" s="14"/>
+      <c r="C90" s="10"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="12">
@@ -1594,7 +1607,7 @@
         <v>86.0</v>
       </c>
       <c r="B91" s="9"/>
-      <c r="C91" s="14"/>
+      <c r="C91" s="10"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
       <c r="F91" s="12">
@@ -1607,7 +1620,7 @@
         <v>87.0</v>
       </c>
       <c r="B92" s="9"/>
-      <c r="C92" s="14"/>
+      <c r="C92" s="10"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
       <c r="F92" s="12">
@@ -1620,7 +1633,7 @@
         <v>88.0</v>
       </c>
       <c r="B93" s="9"/>
-      <c r="C93" s="14"/>
+      <c r="C93" s="10"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="12">
@@ -1633,7 +1646,7 @@
         <v>89.0</v>
       </c>
       <c r="B94" s="9"/>
-      <c r="C94" s="14"/>
+      <c r="C94" s="10"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="12">
@@ -1646,7 +1659,7 @@
         <v>90.0</v>
       </c>
       <c r="B95" s="9"/>
-      <c r="C95" s="14"/>
+      <c r="C95" s="10"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
       <c r="F95" s="12">
@@ -1659,7 +1672,7 @@
         <v>91.0</v>
       </c>
       <c r="B96" s="9"/>
-      <c r="C96" s="14"/>
+      <c r="C96" s="10"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
       <c r="F96" s="12">
@@ -1672,7 +1685,7 @@
         <v>92.0</v>
       </c>
       <c r="B97" s="9"/>
-      <c r="C97" s="14"/>
+      <c r="C97" s="10"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="12">
@@ -1685,7 +1698,7 @@
         <v>93.0</v>
       </c>
       <c r="B98" s="9"/>
-      <c r="C98" s="14"/>
+      <c r="C98" s="10"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
       <c r="F98" s="12">
@@ -1698,7 +1711,7 @@
         <v>94.0</v>
       </c>
       <c r="B99" s="9"/>
-      <c r="C99" s="14"/>
+      <c r="C99" s="10"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
       <c r="F99" s="12">
@@ -1711,7 +1724,7 @@
         <v>95.0</v>
       </c>
       <c r="B100" s="9"/>
-      <c r="C100" s="14"/>
+      <c r="C100" s="10"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
       <c r="F100" s="12">
@@ -1724,7 +1737,7 @@
         <v>96.0</v>
       </c>
       <c r="B101" s="9"/>
-      <c r="C101" s="14"/>
+      <c r="C101" s="10"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
       <c r="F101" s="12">
@@ -1737,7 +1750,7 @@
         <v>97.0</v>
       </c>
       <c r="B102" s="9"/>
-      <c r="C102" s="14"/>
+      <c r="C102" s="10"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
       <c r="F102" s="12">
@@ -1750,7 +1763,7 @@
         <v>98.0</v>
       </c>
       <c r="B103" s="9"/>
-      <c r="C103" s="14"/>
+      <c r="C103" s="10"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
       <c r="F103" s="12">
@@ -1763,7 +1776,7 @@
         <v>99.0</v>
       </c>
       <c r="B104" s="9"/>
-      <c r="C104" s="14"/>
+      <c r="C104" s="10"/>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
       <c r="F104" s="12">
@@ -1776,7 +1789,7 @@
         <v>100.0</v>
       </c>
       <c r="B105" s="9"/>
-      <c r="C105" s="14"/>
+      <c r="C105" s="10"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
       <c r="F105" s="12">
@@ -1785,7 +1798,7 @@
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="15"/>
+      <c r="A106" s="14"/>
     </row>
     <row r="107" ht="15.75" customHeight="1"/>
     <row r="108" ht="15.75" customHeight="1"/>
@@ -2691,11 +2704,11 @@
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Digite uma data válida (DD/MM/AAAA" sqref="C6:C105">
       <formula1>OR(NOT(ISERROR(DATEVALUE(C6))), AND(ISNUMBER(C6), LEFT(CELL("format", C6))="D"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Clique e digite um valor da lista de itens" sqref="E6:E105">
-      <formula1>"Normal,Isento,Serviço"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D6:D105">
       <formula1>"Mas,Fem"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Clique e digite um valor da lista de itens" sqref="E6:E105">
+      <formula1>"Normal,Participação,Isento,Serviço"</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -2714,22 +2727,21 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.63"/>
     <col customWidth="1" min="2" max="2" width="15.25"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>200.0</v>
       </c>
     </row>
@@ -2738,18 +2750,25 @@
         <v>12</v>
       </c>
       <c r="B3" s="15">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="14">
         <v>130.0</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="15">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="16">
         <v>0.0</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>

</xml_diff>